<commit_message>
Added test scripts for One Time Survey and deleted some reports
</commit_message>
<xml_diff>
--- a/Test Data/Input.xlsx
+++ b/Test Data/Input.xlsx
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="232">
   <si>
     <t>Login</t>
   </si>
@@ -402,6 +402,9 @@
     <t>Jobseeker(Other Information) About Other Information</t>
   </si>
   <si>
+    <t>Employer(Approve Jobseeker) Approve Jobseeker Application Message</t>
+  </si>
+  <si>
     <t>Oh Jobs PH Test Data</t>
   </si>
   <si>
@@ -447,124 +450,133 @@
     <t>qwertyui</t>
   </si>
   <si>
+    <t>Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Aenean commodo ligula eget dolor.</t>
+  </si>
+  <si>
+    <t>09123456789,09789456123</t>
+  </si>
+  <si>
+    <t>11:00 AM - 08:00 PM</t>
+  </si>
+  <si>
+    <t>6546380</t>
+  </si>
+  <si>
+    <t>https://www.weboutsourcing-gateway.com/</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Saving changes to your profile...</t>
+  </si>
+  <si>
+    <t>IT Application Support</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>NCR</t>
+  </si>
+  <si>
+    <t>Metro Manila</t>
+  </si>
+  <si>
+    <t>Pasig</t>
+  </si>
+  <si>
+    <t>One Corporate Center, Ortigas Center Pasig City</t>
+  </si>
+  <si>
+    <t>20,000</t>
+  </si>
+  <si>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>Installing and configuring computer hardware, software, systems, networks, printers and scanners</t>
+  </si>
+  <si>
+    <t>1 Year or less</t>
+  </si>
+  <si>
+    <t>Bachelor's / College Degree</t>
+  </si>
+  <si>
+    <t>Hardware and Software Troubleshooting, QA Testing</t>
+  </si>
+  <si>
+    <t>IT Jobs, Fresh Grad</t>
+  </si>
+  <si>
+    <t>Submitting your job post...,Your Job has been submitted. Please wait for Oh! Jobs approval.</t>
+  </si>
+  <si>
+    <t>info@ohjobs.ph</t>
+  </si>
+  <si>
+    <t>secret123Q</t>
+  </si>
+  <si>
+    <t>Sending email notification to Paul Solution ,You have successfully approved the job. The employer will be notified of this action.</t>
+  </si>
+  <si>
+    <t>Aron Paul</t>
+  </si>
+  <si>
+    <t>Braza</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>May,28,1998</t>
+  </si>
+  <si>
+    <t>aronpaulbraza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating your Oh Jobs account...Please wait.  ,Your Oh! Jobs PH account has been successfully created! Check your email and confirm to activate your account.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have successfully logged in  </t>
+  </si>
+  <si>
+    <t>Juan Pablo</t>
+  </si>
+  <si>
+    <t>Dela Cruz</t>
+  </si>
+  <si>
+    <t>Jan/07/1992</t>
+  </si>
+  <si>
+    <t>Region III,Bulacan,Malolos</t>
+  </si>
+  <si>
+    <t>00123 Malolos, Bulacan</t>
+  </si>
+  <si>
+    <t>Experienced Level</t>
+  </si>
+  <si>
+    <t>College Graduate</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>09789456123</t>
+  </si>
+  <si>
     <t>Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Aenean commodo ligula eget dolor. Aenean massa. Cum sociis natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus. Donec quam felis, ultricies nec, pellentesque eu, pretium quis, sem. Nulla consequat massa quis enim. Donec pede justo, fringilla vel, aliquet nec, vulputate eget, arcu. In enim justo, rhoncus ut, imperdiet a, venenatis vitae, justo. Nullam dictum felis eu pede mollis pretium. Integer tincidunt. Cras dapibus. Vivamus elementum semper nisi. Aenean vulputate eleifend tellus. Aenean leo ligula, porttitor eu, consequat vitae, eleifend ac, enim. Aliquam lorem ante, dapibus in, viverra quis, feugiat a,</t>
-  </si>
-  <si>
-    <t>09123456789,09789456123</t>
-  </si>
-  <si>
-    <t>11:00 AM - 08:00 PM</t>
-  </si>
-  <si>
-    <t>https://www.weboutsourcing-gateway.com/</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Tokyo, Japan</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>Saving changes to your profile...</t>
-  </si>
-  <si>
-    <t>IT Application Support</t>
-  </si>
-  <si>
-    <t>NCR</t>
-  </si>
-  <si>
-    <t>Metro Manila</t>
-  </si>
-  <si>
-    <t>Pasig</t>
-  </si>
-  <si>
-    <t>One Corporate Center, Ortigas Center Pasig City</t>
-  </si>
-  <si>
-    <t>20,000</t>
-  </si>
-  <si>
-    <t>Full Time</t>
-  </si>
-  <si>
-    <t>Installing and configuring computer hardware, software, systems, networks, printers and scanners</t>
-  </si>
-  <si>
-    <t>1 Year or less</t>
-  </si>
-  <si>
-    <t>Bachelor's / College Degree</t>
-  </si>
-  <si>
-    <t>Hardware and Software Troubleshooting, QA Testing</t>
-  </si>
-  <si>
-    <t>IT Jobs, Fresh Grad</t>
-  </si>
-  <si>
-    <t>Submitting your job post...,Your Job has been submitted. Please wait for Oh! Jobs approval.</t>
-  </si>
-  <si>
-    <t>info@ohjobs.ph</t>
-  </si>
-  <si>
-    <t>secret123Q</t>
-  </si>
-  <si>
-    <t>Sending email notification to Paul Solution ,You have successfully approved the job. The employer will be notified of this action.</t>
-  </si>
-  <si>
-    <t>Aron Paul</t>
-  </si>
-  <si>
-    <t>Braza</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>May,28,1998</t>
-  </si>
-  <si>
-    <t>aronpaulbraza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creating your Oh Jobs account...Please wait.  ,Your Oh! Jobs PH account has been successfully created! Check your email and confirm to activate your account.   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have successfully logged in  </t>
-  </si>
-  <si>
-    <t>Juan Pablo</t>
-  </si>
-  <si>
-    <t>Dela Cruz</t>
-  </si>
-  <si>
-    <t>Jan/07/1992</t>
-  </si>
-  <si>
-    <t>Region III,Bulacan,Malolos</t>
-  </si>
-  <si>
-    <t>00123 Malolos, Bulacan</t>
-  </si>
-  <si>
-    <t>Experienced Level</t>
-  </si>
-  <si>
-    <t>College Graduate</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>09789456123</t>
   </si>
   <si>
     <t>Bachelor of Science in Information Technology</t>
@@ -608,6 +620,9 @@
   <si>
     <t>Learn how to locate webelement.
 Create a page object model.</t>
+  </si>
+  <si>
+    <t>We received your application for the [Job Title] position and are interested in discussing your qualifications further. We would like to invite you to interview at our office to discuss the job requirements and learn more about you.</t>
   </si>
   <si>
     <t>End</t>
@@ -840,11 +855,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -893,44 +908,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -945,33 +923,32 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -983,9 +960,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1000,7 +977,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1092,13 +1107,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1116,7 +1131,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1128,43 +1239,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1176,61 +1275,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1242,37 +1287,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1301,26 +1316,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1344,22 +1350,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1375,6 +1375,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1401,13 +1416,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1419,62 +1434,62 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1483,64 +1498,64 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1622,7 +1637,7 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" quotePrefix="1"/>
@@ -1952,7 +1967,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AS2" sqref="AS2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.78095238095238" defaultRowHeight="15"/>
@@ -2022,7 +2037,7 @@
     <col min="133" max="16384" width="8.78095238095238" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" spans="1:132">
+    <row r="1" ht="60" spans="1:132">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2276,7 +2291,9 @@
       <c r="CI1" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="CJ1" s="12"/>
+      <c r="CJ1" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="CK1" s="12"/>
       <c r="CL1" s="12"/>
       <c r="CM1" s="12"/>
@@ -2324,261 +2341,263 @@
     </row>
     <row r="2" s="11" customFormat="1" ht="409.5" spans="1:132">
       <c r="A2" s="13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="17"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L2" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="X2" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z2" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA2" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB2" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC2" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE2" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF2" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG2" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH2" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI2" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ2" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK2" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="AL2" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM2" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN2" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP2" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="M2" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="P2" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="W2" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="X2" s="29">
-        <v>123456789</v>
-      </c>
-      <c r="Y2" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z2" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA2" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB2" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC2" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD2" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE2" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF2" s="28">
-        <v>10</v>
-      </c>
-      <c r="AG2" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH2" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI2" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ2" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK2" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="AL2" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="AM2" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="AN2" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="AO2" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="AP2" s="29" t="s">
-        <v>90</v>
-      </c>
       <c r="AQ2" s="29" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AR2" s="14" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AS2" s="33">
         <f ca="1">(TODAY())</f>
-        <v>43896</v>
+        <v>43901</v>
       </c>
       <c r="AT2" s="33">
         <f ca="1">(TODAY()+DAY(30))</f>
-        <v>43926</v>
+        <v>43931</v>
       </c>
       <c r="AU2" s="32" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AV2" s="14"/>
       <c r="AW2" s="16" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AX2" s="18" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AY2" s="18" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AZ2" s="18" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="BA2" s="28" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BB2" s="29" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="BC2" s="29" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="BD2" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="BE2" s="14" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="BF2" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BG2" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BH2" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BI2" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ2" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="BK2" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL2" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="BM2" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="BI2" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="BJ2" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="BK2" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="BL2" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="BM2" s="18" t="s">
-        <v>124</v>
-      </c>
       <c r="BN2" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BO2" s="29" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="BP2" s="24" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="BQ2" s="24" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="BR2" s="24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="BS2" s="24" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="BT2" s="24" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="BU2" s="24" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="BV2" s="24" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="BW2" s="24" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="BX2" s="24" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="BY2" s="28" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="BZ2" s="24" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="CA2" s="24" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="CB2" s="24" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="CC2" s="24" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="CD2" s="24" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="CE2" s="24" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="CF2" s="24" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="CG2" s="24" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="CH2" s="24" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="CI2" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="CJ2" s="24"/>
+        <v>155</v>
+      </c>
+      <c r="CJ2" s="24" t="s">
+        <v>156</v>
+      </c>
       <c r="CK2" s="24"/>
       <c r="CL2" s="24"/>
       <c r="CM2" s="24"/>
@@ -3430,7 +3449,7 @@
     </row>
     <row r="9" spans="1:61">
       <c r="A9" s="25" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -3495,11 +3514,11 @@
     </row>
     <row r="10" spans="1:61">
       <c r="A10" s="12" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -3562,11 +3581,11 @@
     </row>
     <row r="11" spans="1:61">
       <c r="A11" s="13" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="15" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -22142,639 +22161,639 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="6" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="8" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="8" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="7" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="7" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:5">
       <c r="A27" s="4" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="8" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="7" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="4" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="4" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="4" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="10" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="4" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="4" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="4" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="7" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="7" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="7" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="4" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" ht="17.25" customHeight="1" spans="1:5">
       <c r="A47" s="4" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>